<commit_message>
Fixes to week 8 errors
Fixing an error in calculations of the solved spreadsheet and the first example in the slides
</commit_message>
<xml_diff>
--- a/week 8 (Lab 4- Binomials and AIC)/Binomial AIC Lab_solved.xlsx
+++ b/week 8 (Lab 4- Binomials and AIC)/Binomial AIC Lab_solved.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umainesystem-my.sharepoint.com/personal/liam_berigan_maine_edu/Documents/MaineAnalysis/WLE411/week 8 (Lab 4- Binomials and AIC)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="11_6E4039C9E53DCDFFEB9DD46C33C66400902D7DBE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD70A2C9-57B3-4B06-B65E-98462F7D9597}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="11_6E4039C9E53DCDFFEB9DD46C33C66400902D7DBE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A68234A4-EDC0-423B-AD16-A79A9D428099}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lab Exercise" sheetId="1" r:id="rId1"/>
@@ -519,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,20 +874,20 @@
         <v>9</v>
       </c>
       <c r="B16" s="4">
-        <f>-2*LN(B2) + (2*1*(1/(20-1-1)))</f>
-        <v>33.571323468800728</v>
+        <f>-2*LN(B2) + (2*1*(20/(20-1-1)))</f>
+        <v>35.682434579911835</v>
       </c>
       <c r="C16" s="4">
         <f>B16-MIN($B$16:$B$24)</f>
-        <v>30.027343802012059</v>
+        <v>30.027343802012055</v>
       </c>
       <c r="D16" s="4">
         <f>EXP(-(C16/2))</f>
-        <v>3.017485141754152E-7</v>
+        <v>3.0174851417541573E-7</v>
       </c>
       <c r="E16" s="4">
         <f>D16/$G$25</f>
-        <v>1.138729739286906E-7</v>
+        <v>1.1387297392869081E-7</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -895,8 +895,8 @@
         <v>17</v>
       </c>
       <c r="B17" s="4">
-        <f t="shared" ref="B17:B24" si="7">-2*LN(B3) + (2*1*(1/(20-1-1)))</f>
-        <v>18.820319705864176</v>
+        <f t="shared" ref="B17:B24" si="7">-2*LN(B3) + (2*1*(20/(20-1-1)))</f>
+        <v>20.931430816975286</v>
       </c>
       <c r="C17" s="4">
         <f t="shared" ref="C17:C24" si="8">B17-MIN($B$16:$B$24)</f>
@@ -908,7 +908,7 @@
       </c>
       <c r="E17" s="4">
         <f t="shared" ref="E17:E24" si="10">D17/$G$25</f>
-        <v>1.8178599904861034E-4</v>
+        <v>1.8178599904861037E-4</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -917,19 +917,19 @@
       </c>
       <c r="B18" s="4">
         <f t="shared" si="7"/>
-        <v>11.225659393260598</v>
+        <v>13.33677050437171</v>
       </c>
       <c r="C18" s="4">
         <f t="shared" si="8"/>
-        <v>7.681679726471927</v>
+        <v>7.6816797264719288</v>
       </c>
       <c r="D18" s="4">
         <f t="shared" si="9"/>
-        <v>2.1475557237863513E-2</v>
+        <v>2.1475557237863496E-2</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" si="10"/>
-        <v>8.1043831355196091E-3</v>
+        <v>8.1043831355196039E-3</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -938,15 +938,15 @@
       </c>
       <c r="B19" s="4">
         <f t="shared" si="7"/>
-        <v>6.7877005316539831</v>
+        <v>8.8988116427650947</v>
       </c>
       <c r="C19" s="4">
         <f t="shared" si="8"/>
-        <v>3.2437208648653129</v>
+        <v>3.2437208648653133</v>
       </c>
       <c r="D19" s="4">
         <f t="shared" si="9"/>
-        <v>0.19753086419753108</v>
+        <v>0.19753086419753105</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" si="10"/>
@@ -959,19 +959,19 @@
       </c>
       <c r="B20" s="4">
         <f t="shared" si="7"/>
-        <v>4.3494002088162258</v>
+        <v>6.4605113199273374</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" si="8"/>
-        <v>0.80542054202755553</v>
+        <v>0.80542054202755597</v>
       </c>
       <c r="D20" s="4">
         <f t="shared" si="9"/>
-        <v>0.66850575676330959</v>
+        <v>0.66850575676330937</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" si="10"/>
-        <v>0.25227875212281708</v>
+        <v>0.25227875212281703</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -980,7 +980,7 @@
       </c>
       <c r="B21" s="4">
         <f t="shared" si="7"/>
-        <v>3.5439796667886703</v>
+        <v>5.6550907778997814</v>
       </c>
       <c r="C21" s="4">
         <f t="shared" si="8"/>
@@ -992,7 +992,7 @@
       </c>
       <c r="E21" s="4">
         <f t="shared" si="10"/>
-        <v>0.37737708250153279</v>
+        <v>0.37737708250153285</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1001,15 +1001,15 @@
       </c>
       <c r="B22" s="4">
         <f t="shared" si="7"/>
-        <v>4.4472765101629665</v>
+        <v>6.5583876212740781</v>
       </c>
       <c r="C22" s="4">
         <f t="shared" si="8"/>
-        <v>0.90329684337429628</v>
+        <v>0.90329684337429672</v>
       </c>
       <c r="D22" s="4">
         <f t="shared" si="9"/>
-        <v>0.63657793738407831</v>
+        <v>0.6365779373840782</v>
       </c>
       <c r="E22" s="4">
         <f t="shared" si="10"/>
@@ -1022,7 +1022,7 @@
       </c>
       <c r="B23" s="4">
         <f t="shared" si="7"/>
-        <v>7.7299648169050554</v>
+        <v>9.841075928016167</v>
       </c>
       <c r="C23" s="4">
         <f t="shared" si="8"/>
@@ -1034,7 +1034,7 @@
       </c>
       <c r="E23" s="4">
         <f t="shared" si="10"/>
-        <v>4.6537215756444116E-2</v>
+        <v>4.6537215756444122E-2</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1043,7 +1043,7 @@
       </c>
       <c r="B24" s="4">
         <f t="shared" si="7"/>
-        <v>15.993526850110978</v>
+        <v>18.104637961222089</v>
       </c>
       <c r="C24" s="4">
         <f t="shared" si="8"/>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="E24" s="4">
         <f t="shared" si="10"/>
-        <v>7.4712058194613764E-4</v>
+        <v>7.4712058194613775E-4</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1067,7 +1067,7 @@
       </c>
       <c r="G25" s="4">
         <f>SUM(D16:D24)</f>
-        <v>2.6498694445652733</v>
+        <v>2.6498694445652728</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1097,8 +1097,8 @@
         <v>9</v>
       </c>
       <c r="B28" s="4">
-        <f>-2*LN(C2) + (2*1*(1/(20-1-1)))</f>
-        <v>64.278631654746931</v>
+        <f>-2*LN(C2) + (2*1*(40/(40-1-1)))</f>
+        <v>66.272783701530557</v>
       </c>
       <c r="C28" s="4">
         <f>B28-MIN($B$28:$B$36)</f>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="E28" s="4">
         <f>D28/$G$37</f>
-        <v>4.7750731521251745E-14</v>
+        <v>4.7750731521251751E-14</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1118,8 +1118,8 @@
         <v>17</v>
       </c>
       <c r="B29" s="4">
-        <f t="shared" ref="B29:B36" si="11">-2*LN(C3) + (2*1*(1/(20-1-1)))</f>
-        <v>34.776624128873827</v>
+        <f t="shared" ref="B29:B36" si="11">-2*LN(C3) + (2*1*(40/(40-1-1)))</f>
+        <v>36.770776175657453</v>
       </c>
       <c r="C29" s="4">
         <f t="shared" ref="C29:C36" si="12">B29-MIN($B$28:$B$36)</f>
@@ -1140,7 +1140,7 @@
       </c>
       <c r="B30" s="4">
         <f t="shared" si="11"/>
-        <v>19.587303503666671</v>
+        <v>21.581455550450297</v>
       </c>
       <c r="C30" s="4">
         <f t="shared" si="12"/>
@@ -1152,7 +1152,7 @@
       </c>
       <c r="E30" s="4">
         <f t="shared" si="14"/>
-        <v>2.4186812152010516E-4</v>
+        <v>2.4186812152010519E-4</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1161,7 +1161,7 @@
       </c>
       <c r="B31" s="4">
         <f t="shared" si="11"/>
-        <v>10.711385780453444</v>
+        <v>12.70553782723707</v>
       </c>
       <c r="C31" s="4">
         <f t="shared" si="12"/>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="E31" s="4">
         <f t="shared" si="14"/>
-        <v>2.0462546350625551E-2</v>
+        <v>2.0462546350625554E-2</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1182,7 +1182,7 @@
       </c>
       <c r="B32" s="4">
         <f t="shared" si="11"/>
-        <v>5.8347851347779276</v>
+        <v>7.8289371815615532</v>
       </c>
       <c r="C32" s="4">
         <f t="shared" si="12"/>
@@ -1194,7 +1194,7 @@
       </c>
       <c r="E32" s="4">
         <f t="shared" si="14"/>
-        <v>0.23436893772468398</v>
+        <v>0.23436893772468401</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1203,7 +1203,7 @@
       </c>
       <c r="B33" s="4">
         <f t="shared" si="11"/>
-        <v>4.2239440507228156</v>
+        <v>6.2180960975064412</v>
       </c>
       <c r="C33" s="4">
         <f t="shared" si="12"/>
@@ -1215,7 +1215,7 @@
       </c>
       <c r="E33" s="4">
         <f t="shared" si="14"/>
-        <v>0.52443268205646143</v>
+        <v>0.52443268205646154</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1224,19 +1224,19 @@
       </c>
       <c r="B34" s="4">
         <f t="shared" si="11"/>
-        <v>6.0305377374714082</v>
+        <v>8.0246897842550347</v>
       </c>
       <c r="C34" s="4">
         <f t="shared" si="12"/>
-        <v>1.8065936867485926</v>
+        <v>1.8065936867485934</v>
       </c>
       <c r="D34" s="4">
         <f t="shared" si="13"/>
-        <v>0.40523147036416751</v>
+        <v>0.40523147036416735</v>
       </c>
       <c r="E34" s="4">
         <f t="shared" si="14"/>
-        <v>0.21251662685676384</v>
+        <v>0.21251662685676376</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1245,7 +1245,7 @@
       </c>
       <c r="B35" s="4">
         <f t="shared" si="11"/>
-        <v>12.595914350955587</v>
+        <v>14.590066397739212</v>
       </c>
       <c r="C35" s="4">
         <f t="shared" si="12"/>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="B36" s="4">
         <f t="shared" si="11"/>
-        <v>29.123038417367432</v>
+        <v>31.117190464151058</v>
       </c>
       <c r="C36" s="4">
         <f t="shared" si="12"/>
@@ -1278,7 +1278,7 @@
       </c>
       <c r="E36" s="4">
         <f t="shared" si="14"/>
-        <v>2.0555124173412176E-6</v>
+        <v>2.055512417341218E-6</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1290,7 +1290,7 @@
       </c>
       <c r="G37" s="4">
         <f>SUM(D28:D36)</f>
-        <v>1.9068224277684092</v>
+        <v>1.9068224277684089</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1320,20 +1320,20 @@
         <v>9</v>
       </c>
       <c r="B40" s="4">
-        <f>-2*LN(D2) + (2*1*(1/(20-1-1)))</f>
-        <v>94.707043591425915</v>
+        <f>-2*LN(D2) + (2*1*(60/(60-1-1)))</f>
+        <v>96.664897997556182</v>
       </c>
       <c r="C40" s="4">
         <f>B40-MIN($B$40:$B$48)</f>
-        <v>90.08203140603618</v>
+        <v>90.082031406036165</v>
       </c>
       <c r="D40" s="4">
         <f>EXP(-(C40/2))</f>
-        <v>2.7474855744737099E-20</v>
+        <v>2.7474855744737291E-20</v>
       </c>
       <c r="E40" s="4">
         <f>D40/$G$49</f>
-        <v>1.7541144595212457E-20</v>
+        <v>1.7541144595212578E-20</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1341,8 +1341,8 @@
         <v>17</v>
       </c>
       <c r="B41" s="4">
-        <f t="shared" ref="B41:B48" si="15">-2*LN(D3) + (2*1*(1/(20-1-1)))</f>
-        <v>50.454032302616255</v>
+        <f t="shared" ref="B41:B48" si="15">-2*LN(D3) + (2*1*(60/(60-1-1)))</f>
+        <v>52.411886708746522</v>
       </c>
       <c r="C41" s="4">
         <f t="shared" ref="C41:C48" si="16">B41-MIN($B$40:$B$48)</f>
@@ -1354,7 +1354,7 @@
       </c>
       <c r="E41" s="4">
         <f t="shared" ref="E41:E48" si="18">D41/$G$49</f>
-        <v>7.1363679436800242E-11</v>
+        <v>7.1363679436800229E-11</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1363,7 +1363,7 @@
       </c>
       <c r="B42" s="4">
         <f t="shared" si="15"/>
-        <v>27.670051364805524</v>
+        <v>29.627905770935794</v>
       </c>
       <c r="C42" s="4">
         <f t="shared" si="16"/>
@@ -1375,7 +1375,7 @@
       </c>
       <c r="E42" s="4">
         <f t="shared" si="18"/>
-        <v>6.3234753836744939E-6</v>
+        <v>6.323475383674493E-6</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1384,19 +1384,19 @@
       </c>
       <c r="B43" s="4">
         <f t="shared" si="15"/>
-        <v>14.356174779985682</v>
+        <v>16.314029186115953</v>
       </c>
       <c r="C43" s="4">
         <f t="shared" si="16"/>
-        <v>9.7311625945959399</v>
+        <v>9.7311625945959417</v>
       </c>
       <c r="D43" s="4">
         <f t="shared" si="17"/>
-        <v>7.7073466292589595E-3</v>
+        <v>7.7073466292589526E-3</v>
       </c>
       <c r="E43" s="4">
         <f t="shared" si="18"/>
-        <v>4.9207057873325482E-3</v>
+        <v>4.920705787332543E-3</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1405,19 +1405,19 @@
       </c>
       <c r="B44" s="4">
         <f t="shared" si="15"/>
-        <v>7.0412738114724096</v>
+        <v>8.9991282176026779</v>
       </c>
       <c r="C44" s="4">
         <f t="shared" si="16"/>
-        <v>2.4162616260826679</v>
+        <v>2.416261626082667</v>
       </c>
       <c r="D44" s="4">
         <f t="shared" si="17"/>
-        <v>0.29875518715018728</v>
+        <v>0.2987551871501874</v>
       </c>
       <c r="E44" s="4">
         <f t="shared" si="18"/>
-        <v>0.19073832398101054</v>
+        <v>0.19073832398101059</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1426,7 +1426,7 @@
       </c>
       <c r="B45" s="4">
         <f t="shared" si="15"/>
-        <v>4.6250121853897417</v>
+        <v>6.5828665915200109</v>
       </c>
       <c r="C45" s="4">
         <f t="shared" si="16"/>
@@ -1438,7 +1438,7 @@
       </c>
       <c r="E45" s="4">
         <f t="shared" si="18"/>
-        <v>0.63844355574360101</v>
+        <v>0.6384435557436009</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1447,19 +1447,19 @@
       </c>
       <c r="B46" s="4">
         <f t="shared" si="15"/>
-        <v>7.3349027155126301</v>
+        <v>9.2927571216428984</v>
       </c>
       <c r="C46" s="4">
         <f t="shared" si="16"/>
-        <v>2.7098905301228884</v>
+        <v>2.7098905301228875</v>
       </c>
       <c r="D46" s="4">
         <f t="shared" si="17"/>
-        <v>0.25796141356753904</v>
+        <v>0.25796141356753916</v>
       </c>
       <c r="E46" s="4">
         <f t="shared" si="18"/>
-        <v>0.16469380212270524</v>
+        <v>0.16469380212270526</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -1468,19 +1468,19 @@
       </c>
       <c r="B47" s="4">
         <f t="shared" si="15"/>
-        <v>17.182967635738898</v>
+        <v>19.140822041869168</v>
       </c>
       <c r="C47" s="4">
         <f t="shared" si="16"/>
-        <v>12.557955450349155</v>
+        <v>12.557955450349157</v>
       </c>
       <c r="D47" s="4">
         <f t="shared" si="17"/>
-        <v>1.8753167037162096E-3</v>
+        <v>1.8753167037162078E-3</v>
       </c>
       <c r="E47" s="4">
         <f t="shared" si="18"/>
-        <v>1.197283864465946E-3</v>
+        <v>1.1972838644659447E-3</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -1489,7 +1489,7 @@
       </c>
       <c r="B48" s="4">
         <f t="shared" si="15"/>
-        <v>41.97365373535667</v>
+        <v>43.931508141486937</v>
       </c>
       <c r="C48" s="4">
         <f t="shared" si="16"/>
@@ -1501,7 +1501,7 @@
       </c>
       <c r="E48" s="4">
         <f t="shared" si="18"/>
-        <v>4.9541373373720192E-9</v>
+        <v>4.9541373373720184E-9</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -1513,7 +1513,7 @@
       </c>
       <c r="G49" s="4">
         <f>SUM(D40:D48)</f>
-        <v>1.5663091764397103</v>
+        <v>1.5663091764397106</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -1549,20 +1549,20 @@
         <v>9</v>
       </c>
       <c r="B53" s="4">
-        <f>-2*LN(E2) + (2*1*(1/(20-1-1)))</f>
-        <v>125.01987067795156</v>
+        <f>-2*LN(E2) + (2*1*(80/(80-1-1)))</f>
+        <v>126.96004161812249</v>
       </c>
       <c r="C53" s="4">
         <f>B53-MIN($B$53:$B$61)</f>
-        <v>120.10937520804823</v>
+        <v>120.10937520804822</v>
       </c>
       <c r="D53" s="4">
         <f>EXP(-(C53/2))</f>
-        <v>8.2904968981583044E-27</v>
+        <v>8.2904968981583633E-27</v>
       </c>
       <c r="E53" s="4">
         <f>D53/$G$62</f>
-        <v>6.0705731687350139E-27</v>
+        <v>6.070573168735057E-27</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1570,20 +1570,20 @@
         <v>17</v>
       </c>
       <c r="B54" s="4">
-        <f t="shared" ref="B54:B61" si="19">-2*LN(E3) + (2*1*(1/(20-1-1)))</f>
-        <v>66.015855626205337</v>
+        <f t="shared" ref="B54:B61" si="19">-2*LN(E3) + (2*1*(80/(80-1-1)))</f>
+        <v>67.956026566376266</v>
       </c>
       <c r="C54" s="4">
         <f t="shared" ref="C54:C61" si="20">B54-MIN($B$53:$B$61)</f>
-        <v>61.105360156302012</v>
+        <v>61.105360156302005</v>
       </c>
       <c r="D54" s="4">
         <f t="shared" ref="D54:D61" si="21">EXP(-(C54/2))</f>
-        <v>5.3844287526534102E-14</v>
+        <v>5.3844287526534298E-14</v>
       </c>
       <c r="E54" s="4">
         <f t="shared" ref="E54:E61" si="22">D54/$G$62</f>
-        <v>3.9426549598111907E-14</v>
+        <v>3.9426549598112052E-14</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -1592,19 +1592,19 @@
       </c>
       <c r="B55" s="4">
         <f t="shared" si="19"/>
-        <v>35.637214375791032</v>
+        <v>37.577385315961969</v>
       </c>
       <c r="C55" s="4">
         <f t="shared" si="20"/>
-        <v>30.726718905887711</v>
+        <v>30.726718905887708</v>
       </c>
       <c r="D55" s="4">
         <f t="shared" si="21"/>
-        <v>2.1270503292363038E-7</v>
+        <v>2.1270503292363075E-7</v>
       </c>
       <c r="E55" s="4">
         <f t="shared" si="22"/>
-        <v>1.5574958673561914E-7</v>
+        <v>1.5574958673561943E-7</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="B56" s="4">
         <f t="shared" si="19"/>
-        <v>17.885378929364578</v>
+        <v>19.825549869535518</v>
       </c>
       <c r="C56" s="4">
         <f t="shared" si="20"/>
@@ -1634,7 +1634,7 @@
       </c>
       <c r="B57" s="4">
         <f t="shared" si="19"/>
-        <v>8.1321776380135447</v>
+        <v>10.072348578184485</v>
       </c>
       <c r="C57" s="4">
         <f t="shared" si="20"/>
@@ -1655,7 +1655,7 @@
       </c>
       <c r="B58" s="4">
         <f t="shared" si="19"/>
-        <v>4.9104954699033208</v>
+        <v>6.8506664100742611</v>
       </c>
       <c r="C58" s="4">
         <f t="shared" si="20"/>
@@ -1676,7 +1676,7 @@
       </c>
       <c r="B59" s="4">
         <f t="shared" si="19"/>
-        <v>8.5236828434005059</v>
+        <v>10.463853783571446</v>
       </c>
       <c r="C59" s="4">
         <f t="shared" si="20"/>
@@ -1697,7 +1697,7 @@
       </c>
       <c r="B60" s="4">
         <f t="shared" si="19"/>
-        <v>21.654436070368863</v>
+        <v>23.594607010539804</v>
       </c>
       <c r="C60" s="4">
         <f t="shared" si="20"/>
@@ -1718,7 +1718,7 @@
       </c>
       <c r="B61" s="4">
         <f t="shared" si="19"/>
-        <v>54.708684203192561</v>
+        <v>56.648855143363498</v>
       </c>
       <c r="C61" s="4">
         <f t="shared" si="20"/>
@@ -1755,7 +1755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>

</xml_diff>